<commit_message>
saving for end of day
</commit_message>
<xml_diff>
--- a/leaders.xlsx
+++ b/leaders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:BB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,55 +434,164 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>first_name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>last_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>death_date</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>place_of_birth</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>wikipedia_url</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>start_mandate</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>end_mandate</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>biography</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -491,45 +600,267 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Q57553</t>
+          <t>{'id': 'Q12978', 'first_name': 'Guy', 'last_name': 'Verhofstadt', 'birth_date': '1953-04-11', 'death_date': None, 'place_of_birth': 'Dendermonde', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Guy_Verhofstadt', 'start_mandate': '1999-07-12', 'end_mandate': '2008-03-20'}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mohammed</t>
+          <t>{'id': 'Q12981', 'first_name': 'Yves', 'last_name': 'Leterme', 'birth_date': '1960-10-06', 'death_date': None, 'place_of_birth': 'Wervik', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Yves_Leterme', 'start_mandate': '2009-11-25', 'end_mandate': '2011-12-06'}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>{'id': 'Q12983', 'first_name': 'Herman', 'last_name': 'None', 'birth_date': '1947-10-31', 'death_date': None, 'place_of_birth': 'Etterbeek', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Herman_Van_Rompuy', 'start_mandate': '2008-12-30', 'end_mandate': '2009-11-25'}</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1963-08-21</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>{'id': 'Q14989', 'first_name': 'Léon', 'last_name': 'Delacroix', 'birth_date': '1867-12-27', 'death_date': '1929-10-15', 'place_of_birth': 'Saint-Josse-ten-Noode', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/L%C3%A9on_Delacroix', 'start_mandate': '1918-11-21', 'end_mandate': '1920-11-20'}</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q14990', 'first_name': 'Henry', 'last_name': 'Carton', 'birth_date': '1869-01-31', 'death_date': '1951-05-06', 'place_of_birth': 'Brussels', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Henri_Carton_de_Wiart', 'start_mandate': '1920-11-20', 'end_mandate': '1921-12-16'}</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Rabat</t>
+          <t>{'id': 'Q14991', 'first_name': 'Georges', 'last_name': 'Theunis', 'birth_date': '1873-02-28', 'death_date': '1966-01-04', 'place_of_birth': 'Montegnée', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Georges_Theunis', 'start_mandate': '1934-11-20', 'end_mandate': '1935-03-25'}</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%B3%D8%A7%D8%AF%D8%B3_%D8%A8%D9%86_%D8%A7%D9%84%D8%AD%D8%B3%D9%86</t>
+          <t>{'id': 'Q14992', 'first_name': 'Aloïs', 'last_name': 'Van de Vyvere', 'birth_date': '1871-06-08', 'death_date': '1961-10-22', 'place_of_birth': 'Tielt', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Aloys_Van_de_Vyvere', 'start_mandate': '1925-05-13', 'end_mandate': '1925-06-17'}</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1999-07-23</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
+          <t>{'id': 'Q14993', 'first_name': 'Prosper', 'last_name': 'Poullet', 'birth_date': '1868-03-05', 'death_date': '1937-12-03', 'place_of_birth': 'Leuven', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Prosper_Poullet', 'start_mandate': '1925-06-17', 'end_mandate': '1926-05-20'}</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q14994', 'first_name': 'Henri', 'last_name': 'Jaspar', 'birth_date': '1870-07-28', 'death_date': '1939-02-15', 'place_of_birth': 'Schaerbeek - Schaarbeek', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Henri_Jaspar', 'start_mandate': '1926-05-20', 'end_mandate': '1931-06-06'}</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">محمد السادس بن الحسن الثاني العلوي هو ملك المملكة المغربية منذ عام 1999 والملك الثالث والعشرون للمغرب من سلالة العلويين الفيلاليين تولى الحكم خلفا لوالده الملك الحسن الثاني بعد وفاته وتمت البيعة له ملكا يوم الجمعة 9 ربيع الثاني سنة 1420 هـ الموافق 23 يوليو 1999 بالقصر الملكي بالرباط.
-</t>
+          <t>{'id': 'Q14995', 'first_name': 'Jules', 'last_name': 'None', 'birth_date': '1862-12-03', 'death_date': '1934-07-15', 'place_of_birth': 'Ixelles - Elsene', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jules_Renkin', 'start_mandate': '1931-06-06', 'end_mandate': '1932-10-22'}</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q14996', 'first_name': 'Paul', 'last_name': 'Van Zeeland', 'birth_date': '1893-11-11', 'death_date': '1973-09-22', 'place_of_birth': 'Soignies', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Paul_van_Zeeland', 'start_mandate': '1935-03-25', 'end_mandate': '1937-11-24'}</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q14997', 'first_name': 'Achille', 'last_name': 'Van Acker', 'birth_date': '1898-04-08', 'death_date': '1975-07-10', 'place_of_birth': 'Bruges', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Achiel_Van_Acker', 'start_mandate': '1954-04-23', 'end_mandate': '1958-06-26'}</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q14998', 'first_name': 'Camille', 'last_name': 'Huysmans', 'birth_date': '1871-05-26', 'death_date': '1968-02-25', 'place_of_birth': 'Bilzen', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Camille_Huysmans', 'start_mandate': '1946-08-03', 'end_mandate': '1947-03-20'}</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q14999', 'first_name': 'Gaston', 'last_name': 'Eyskens', 'birth_date': '1905-04-01', 'death_date': '1988-01-03', 'place_of_birth': 'Lier', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Gaston_Eyskens', 'start_mandate': '1968-07-17', 'end_mandate': '1973-01-26'}</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q15002', 'first_name': 'Leo', 'last_name': 'Tindemans', 'birth_date': '1922-04-16', 'death_date': '2014-12-26', 'place_of_birth': 'Zwijndrecht', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Leo_Tindemans', 'start_mandate': '1974-04-25', 'end_mandate': '1978-10-20'}</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q15048', 'first_name': 'Elio', 'last_name': 'Di Rupo', 'birth_date': '1951-07-18', 'death_date': None, 'place_of_birth': 'Morlanwelz', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Elio_Di_Rupo', 'start_mandate': '2011-12-06', 'end_mandate': '2014-10-11'}</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q15056', 'first_name': 'Jean-Luc', 'last_name': 'Dehaene', 'birth_date': '1940-08-07', 'death_date': '2014-05-15', 'place_of_birth': 'Montpellier', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jean-Luc_Dehaene', 'start_mandate': '1992-03-07', 'end_mandate': '1999-07-12'}</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q15956', 'first_name': 'Frans', 'last_name': 'Schollaert', 'birth_date': '1851-08-19', 'death_date': '1917-06-29', 'place_of_birth': 'Wilsele', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Frans_Schollaert', 'start_mandate': '1908-01-09', 'end_mandate': '1911-06-17'}</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q143202', 'first_name': 'Pieter', 'last_name': 'Decker', 'birth_date': '1812-01-25', 'death_date': '1891-01-04', 'place_of_birth': 'Zele', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Pieter_de_Decker', 'start_mandate': '1855-03-30', 'end_mandate': '1857-11-09'}</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q155691', 'first_name': 'Paul-Henri', 'last_name': 'Spaak', 'birth_date': '1899-01-25', 'death_date': '1972-07-31', 'place_of_birth': 'Schaerbeek - Schaarbeek', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Paul-Henri_Spaak', 'start_mandate': '1947-03-20', 'end_mandate': '1949-08-11'}</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q202049', 'first_name': 'Auguste', 'last_name': 'Beernaert', 'birth_date': '1829-07-26', 'death_date': '1912-10-06', 'place_of_birth': 'Ostend', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Auguste_Beernaert', 'start_mandate': '1884-10-26', 'end_mandate': '1894-03-26'}</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q221781', 'first_name': 'Théodore', 'last_name': 'Lefèvre', 'birth_date': '1914-01-17', 'death_date': '1973-09-18', 'place_of_birth': 'Ghent', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Th%C3%A9o_Lef%C3%A8vre', 'start_mandate': '1961-04-25', 'end_mandate': '1965-07-28'}</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q250021', 'first_name': 'Paul', 'last_name': 'None', 'birth_date': '1919-05-22', 'death_date': '2001-01-09', 'place_of_birth': 'Forest', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Paul_Vanden_Boeynants', 'start_mandate': '1978-10-20', 'end_mandate': '1979-04-03'}</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q289570', 'first_name': 'Étienne', 'last_name': 'Gerlache', 'birth_date': '1785-12-26', 'death_date': '1871-02-10', 'place_of_birth': 'Château of Biourge', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Etienne_de_Gerlache', 'start_mandate': '1831-02-27', 'end_mandate': '1831-03-10'}</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q313809', 'first_name': 'Wilfried', 'last_name': 'Martens', 'birth_date': '1936-04-19', 'death_date': '2013-10-09', 'place_of_birth': 'Sleidinge', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Wilfried_Martens', 'start_mandate': '1981-12-17', 'end_mandate': '1992-03-07'}</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q349477', 'first_name': 'Mark', 'last_name': 'Eyskens', 'birth_date': '1933-04-29', 'death_date': None, 'place_of_birth': 'Leuven', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Mark_Eyskens', 'start_mandate': '1981-04-06', 'end_mandate': '1981-12-17'}</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q363942', 'first_name': 'Pierre', 'last_name': 'Harmel', 'birth_date': '1911-03-16', 'death_date': '2009-11-15', 'place_of_birth': 'Uccle', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Pierre_Harmel', 'start_mandate': '1965-07-28', 'end_mandate': '1966-03-19'}</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q442578', 'first_name': 'Hubert', 'last_name': 'Pierlot', 'birth_date': '1883-12-23', 'death_date': '1963-12-13', 'place_of_birth': 'Bertrix', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Hubert_Pierlot', 'start_mandate': '1939-02-22', 'end_mandate': '1945-02-12'}</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q446472', 'first_name': 'Jean-Baptiste', 'last_name': 'Nothomb', 'birth_date': '1805-07-03', 'death_date': '1881-09-16', 'place_of_birth': 'Messancy', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jean-Baptiste_Nothomb', 'start_mandate': '1841-04-13', 'end_mandate': '1845-07-30'}</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q461745', 'first_name': 'Edmond', 'last_name': 'None', 'birth_date': '1915-04-18', 'death_date': '1997-06-15', 'place_of_birth': 'Lantremange', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Edmond_Leburton', 'start_mandate': '1973-01-26', 'end_mandate': '1974-04-25'}</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q461753', 'first_name': 'Jean', 'last_name': 'None', 'birth_date': '1900-04-10', 'death_date': '1977-10-11', 'place_of_birth': 'Frasnes-lez-Gosselies', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jean_Duvieusart', 'start_mandate': '1950-06-08', 'end_mandate': '1950-08-16'}</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q468104', 'first_name': 'Joseph', 'last_name': 'Lebeau', 'birth_date': '1794-01-03', 'death_date': '1865-03-19', 'place_of_birth': 'Huy', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Joseph_Lebeau', 'start_mandate': '1840-04-18', 'end_mandate': '1841-04-13'}</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q468109', 'first_name': 'Charles', 'last_name': 'Rogier', 'birth_date': '1800-08-17', 'death_date': '1885-05-27', 'place_of_birth': 'Saint-Quentin', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Charles_Rogier', 'start_mandate': '1857-11-09', 'end_mandate': '1868-01-03'}</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q472257', 'first_name': 'Barthélemy', 'last_name': 'None', 'birth_date': '1794-02-26', 'death_date': '1874-08-24', 'place_of_birth': 'Kasteel van Schabroek', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Barth%C3%A9lemy_de_Theux_de_Meylandt', 'start_mandate': '1871-12-07', 'end_mandate': '1874-08-21'}</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q472276', 'first_name': 'Felix', 'last_name': 'None', 'birth_date': '1793-04-05', 'death_date': '1862-08-05', 'place_of_birth': 'Pittem', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Felix_de_M%C3%BBelenaere', 'start_mandate': '1831-07-24', 'end_mandate': '1832-10-20'}</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q476596', 'first_name': 'Alexander', 'last_name': 'De Croo', 'birth_date': '1975-11-03', 'death_date': None, 'place_of_birth': 'Vilvoorde', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Alexander_De_Croo', 'start_mandate': '2020-10-01', 'end_mandate': None}</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q527479', 'first_name': 'Henri', 'last_name': 'de Brouckère', 'birth_date': '1801-01-25', 'death_date': '1891-01-25', 'place_of_birth': 'Bruges', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Henri_de_Brouck%C3%A8re', 'start_mandate': '1852-10-31', 'end_mandate': '1855-03-30'}</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q533339', 'first_name': 'Albert', 'last_name': 'None', 'birth_date': '1790-05-26', 'death_date': '1873-05-05', 'place_of_birth': 'Tournai', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Albert_Goblet_d%27Alviella', 'start_mandate': '1832-10-20', 'end_mandate': '1834-08-04'}</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q546727', 'first_name': 'Sylvain', 'last_name': 'Weyer', 'birth_date': '1802-01-19', 'death_date': '1874-05-23', 'place_of_birth': 'Leuven', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Sylvain_Van_de_Weyer', 'start_mandate': '1845-07-30', 'end_mandate': '1846-03-31'}</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q569138', 'first_name': 'Jules', 'last_name': 'Burlet', 'birth_date': '1844-04-10', 'death_date': '1897-03-01', 'place_of_birth': 'Ixelles - Elsene', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jules_de_Burlet', 'start_mandate': '1894-03-26', 'end_mandate': '1896-02-25'}</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q665955', 'first_name': 'Paul-Émile', 'last_name': 'None', 'birth_date': '1872-05-30', 'death_date': '1944-03-03', 'place_of_birth': 'Brussels metropolitan area', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Paul-Emile_Janson', 'start_mandate': '1937-11-24', 'end_mandate': '1938-05-15'}</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q678535', 'first_name': 'Jules', 'last_name': 'Malou', 'birth_date': '1810-10-19', 'death_date': '1886-07-11', 'place_of_birth': 'Ypres', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jules_Malou', 'start_mandate': '1884-06-16', 'end_mandate': '1884-10-26'}</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q705103', 'first_name': 'Charles', 'last_name': 'Broqueville', 'birth_date': '1860-12-04', 'death_date': '1940-09-05', 'place_of_birth': 'Postel', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Charles_de_Broqueville', 'start_mandate': '1932-10-22', 'end_mandate': '1934-11-20'}</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q705111', 'first_name': 'Joseph', 'last_name': 'Pholien', 'birth_date': '1884-12-28', 'death_date': '1968-01-04', 'place_of_birth': 'Liège', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Joseph_Pholien', 'start_mandate': '1950-08-16', 'end_mandate': '1952-01-15'}</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q705128', 'first_name': 'Jean', 'last_name': 'Van Houtte', 'birth_date': '1907-03-17', 'death_date': '1991-05-23', 'place_of_birth': 'Ghent', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jean_Van_Houtte', 'start_mandate': '1952-01-15', 'end_mandate': '1954-04-23'}</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q705791', 'first_name': 'Walthère', 'last_name': 'Frère', 'birth_date': '1812-04-22', 'death_date': '1896-01-02', 'place_of_birth': 'Liège', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Walth%C3%A8re_Fr%C3%A8re-Orban', 'start_mandate': '1878-06-19', 'end_mandate': '1884-06-16'}</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q719483', 'first_name': 'Gérard', 'last_name': 'Cooreman', 'birth_date': '1852-03-25', 'death_date': '1926-12-02', 'place_of_birth': 'Ghent', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Gerard_Cooreman', 'start_mandate': '1918-06-01', 'end_mandate': '1918-11-21'}</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q721772', 'first_name': 'Jules', 'last_name': 'Vandenpeereboom', 'birth_date': '1843-03-18', 'death_date': '1917-03-06', 'place_of_birth': 'Kortrijk', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jules_Vandenpeereboom', 'start_mandate': '1899-01-24', 'end_mandate': '1899-08-05'}</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q721781', 'first_name': 'Paul', 'last_name': 'None', 'birth_date': '1843-05-13', 'death_date': '1913-09-09', 'place_of_birth': 'Ghent', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Paul_de_Smet_de_Naeyer', 'start_mandate': '1899-08-05', 'end_mandate': '1907-05-02'}</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q721798', 'first_name': 'Jules', 'last_name': 'Trooz', 'birth_date': '1857-02-21', 'death_date': '1907-12-31', 'place_of_birth': 'Leuven', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jules_de_Trooz', 'start_mandate': '1907-05-02', 'end_mandate': '1907-12-31'}</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q725589', 'first_name': 'Jules', 'last_name': "d'Anethan", 'birth_date': '1803-04-23', 'death_date': '1888-10-08', 'place_of_birth': 'Brussels metropolitan area', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Jules_Joseph_d%27Anethan', 'start_mandate': '1870-07-02', 'end_mandate': '1871-12-07'}</t>
+        </is>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q950958', 'first_name': 'Charles', 'last_name': 'Michel', 'birth_date': '1975-12-21', 'death_date': None, 'place_of_birth': 'Namur', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Charles_Michel', 'start_mandate': '2014-10-11', 'end_mandate': '2019-10-27'}</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>{'id': 'Q18434995', 'first_name': 'Sophie', 'last_name': 'Wilmès', 'birth_date': '1975-01-15', 'death_date': None, 'place_of_birth': 'Ixelles - Elsene', 'wikipedia_url': 'https://nl.wikipedia.org/wiki/Sophie_Wilm%C3%A8s', 'start_mandate': '2019-10-27', 'end_mandate': '2020-10-01'}</t>
         </is>
       </c>
     </row>
@@ -539,55 +870,181 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Q69103</t>
+          <t>{'id': 'Q157', 'first_name': 'François', 'last_name': 'Hollande', 'birth_date': '1954-08-12', 'death_date': None, 'place_of_birth': 'Rouen', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Fran%C3%A7ois_Hollande', 'start_mandate': '2012-05-15', 'end_mandate': '2017-05-14'}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hassan</t>
+          <t>{'id': 'Q329', 'first_name': 'Nicolas', 'last_name': 'Sarkozy', 'birth_date': '1955-01-28', 'death_date': None, 'place_of_birth': 'Paris', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Nicolas_Sarkozy', 'start_mandate': '2007-05-16', 'end_mandate': '2012-05-15'}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>{'id': 'Q2038', 'first_name': 'François', 'last_name': 'Mitterrand', 'birth_date': '1916-10-26', 'death_date': '1996-01-08', 'place_of_birth': 'Jarnac', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Fran%C3%A7ois_Mitterrand', 'start_mandate': '1981-05-21', 'end_mandate': '1995-05-17'}</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1929-07-09</t>
+          <t>{'id': 'Q2042', 'first_name': 'Charles', 'last_name': 'de Gaulle', 'birth_date': '1890-11-22', 'death_date': '1970-11-09', 'place_of_birth': 'Lille', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Charles_de_Gaulle', 'start_mandate': '1959-01-08', 'end_mandate': '1969-04-28'}</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1999-07-20</t>
+          <t>{'id': 'Q2105', 'first_name': 'Jacques', 'last_name': 'Chirac', 'birth_date': '1932-11-29', 'death_date': '2019-09-26', 'place_of_birth': '5th arrondissement of Paris', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Jacques_Chirac', 'start_mandate': '1995-05-17', 'end_mandate': '2007-05-16'}</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Rabat</t>
+          <t>{'id': 'Q2124', 'first_name': 'Valéry', 'last_name': "Giscard d'Estaing", 'birth_date': '1926-02-02', 'death_date': '2020-12-02', 'place_of_birth': 'Koblenz', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Val%C3%A9ry_Giscard_d%27Estaing', 'start_mandate': '1974-05-27', 'end_mandate': '1981-05-21'}</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/%D8%A7%D9%84%D8%AD%D8%B3%D9%86_%D8%A7%D9%84%D8%AB%D8%A7%D9%86%D9%8A_%D8%A8%D9%86_%D9%85%D8%AD%D9%85%D8%AF</t>
+          <t>{'id': 'Q2185', 'first_name': 'Georges', 'last_name': 'Pompidou', 'birth_date': '1911-07-05', 'death_date': '1974-04-02', 'place_of_birth': 'Montboudif', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Georges_Pompidou', 'start_mandate': '1969-06-20', 'end_mandate': '1974-04-02'}</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1961-02-26</t>
+          <t>{'id': 'Q5738', 'first_name': 'Adolphe', 'last_name': 'Thiers', 'birth_date': '1797-04-15', 'death_date': '1877-09-03', 'place_of_birth': 'Marseille', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Adolphe_Thiers', 'start_mandate': '1871-08-31', 'end_mandate': '1873-05-24'}</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1999-07-23</t>
+          <t>{'id': 'Q7721', 'first_name': 'Napoléon', 'last_name': 'Bonaparte', 'birth_date': '1808-04-20', 'death_date': '1873-01-09', 'place_of_birth': 'Paris', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Napol%C3%A9on_III', 'start_mandate': '1848-12-20', 'end_mandate': '1852-12-02'}</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">الحسن الثاني بن محمد بن يوسف العلوي ثاني ملوك المملكة المغربية بعد الإستقلال والملك الثاني والعشرين للمغرب من سلالة العلويين الفيلاليين تولى حكم المملكة المغربية خلفا لوالده الملك محمد الخامس في 26 فبراير 1961 وحتى وفاته في 20 يوليو 1999. ينتمي الملك الحسن الثاني إلى السلالة العلوية التي تعود في نسبها إلى الحسن بن علي بن أبي طالب وتحكم المغرب منذ عام 1666 ميلادية ويلقب الحاكم منهم بأمير المؤمنين.
-</t>
-        </is>
-      </c>
+          <t>{'id': 'Q12680', 'first_name': 'Paul', 'last_name': 'Doumer', 'birth_date': '1857-03-22', 'death_date': '1932-05-07', 'place_of_birth': 'Aurillac', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Paul_Doumer', 'start_mandate': '1931-06-13', 'end_mandate': '1932-05-07'}</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q12950', 'first_name': 'Alain', 'last_name': 'Poher', 'birth_date': '1909-04-17', 'death_date': '1996-12-09', 'place_of_birth': 'Ablon-sur-Seine', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Alain_Poher', 'start_mandate': '1969-04-28', 'end_mandate': '1969-06-20'}</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q158749', 'first_name': 'Albert', 'last_name': 'Lebrun', 'birth_date': '1871-08-29', 'death_date': '1950-03-06', 'place_of_birth': 'Mercy-le-Haut', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Albert_Lebrun', 'start_mandate': '1932-05-10', 'end_mandate': '1940-07-11'}</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q158768', 'first_name': 'René', 'last_name': 'Coty', 'birth_date': '1882-03-20', 'death_date': '1962-11-22', 'place_of_birth': 'Le Havre', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Ren%C3%A9_Coty', 'start_mandate': '1954-01-16', 'end_mandate': '1959-01-08'}</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q158772', 'first_name': 'Vincent', 'last_name': 'Auriol', 'birth_date': '1884-08-27', 'death_date': '1966-01-01', 'place_of_birth': 'Revel', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Vincent_Auriol', 'start_mandate': '1947-01-16', 'end_mandate': '1954-01-16'}</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q158838', 'first_name': 'Patrice', 'last_name': 'de Mac Mahon', 'birth_date': '1808-06-13', 'death_date': '1893-10-17', 'place_of_birth': 'Sully', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Patrice_de_Mac_Mahon', 'start_mandate': '1873-05-24', 'end_mandate': '1879-01-30'}</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q169502', 'first_name': 'Émile', 'last_name': 'Loubet', 'birth_date': '1838-12-31', 'death_date': '1929-12-20', 'place_of_birth': 'Marsanne', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/%C3%89mile_Loubet', 'start_mandate': '1899-02-18', 'end_mandate': '1906-02-18'}</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q191974', 'first_name': 'Raymond', 'last_name': 'Poincaré', 'birth_date': '1860-08-20', 'death_date': '1934-10-15', 'place_of_birth': 'Bar-le-Duc', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Raymond_Poincar%C3%A9', 'start_mandate': '1913-02-18', 'end_mandate': '1920-02-18'}</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q215778', 'first_name': 'Marie', 'last_name': 'Carnot', 'birth_date': '1837-08-11', 'death_date': '1894-06-25', 'place_of_birth': 'Limoges', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Sadi_Carnot_(homme_d%27%C3%89tat)', 'start_mandate': '1887-12-03', 'end_mandate': '1894-06-25'}</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q274540', 'first_name': 'Alexandre', 'last_name': 'Millerand', 'birth_date': '1859-02-10', 'death_date': '1943-04-06', 'place_of_birth': 'Paris', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Alexandre_Millerand', 'start_mandate': '1920-09-23', 'end_mandate': '1924-06-11'}</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q296064', 'first_name': 'Gaston', 'last_name': 'Doumergue', 'birth_date': '1863-08-01', 'death_date': '1937-06-18', 'place_of_birth': 'Aigues-Vives', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Gaston_Doumergue', 'start_mandate': '1924-06-13', 'end_mandate': '1931-06-13'}</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q296076', 'first_name': 'Félix', 'last_name': 'Faure', 'birth_date': '1841-01-30', 'death_date': '1899-02-16', 'place_of_birth': 'Paris', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/F%C3%A9lix_Faure', 'start_mandate': '1895-01-17', 'end_mandate': '1899-02-16'}</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q296083', 'first_name': 'Jules', 'last_name': 'Grévy', 'birth_date': '1807-08-15', 'death_date': '1891-09-09', 'place_of_birth': 'Mont-sous-Vaudrey', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Jules_Gr%C3%A9vy', 'start_mandate': '1879-01-30', 'end_mandate': '1887-12-02'}</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q296673', 'first_name': 'Clément', 'last_name': 'Fallières', 'birth_date': '1841-11-06', 'death_date': '1931-06-22', 'place_of_birth': 'Mézin', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Armand_Falli%C3%A8res', 'start_mandate': '1906-02-18', 'end_mandate': '1913-02-18'}</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q309995', 'first_name': 'Paul', 'last_name': 'Deschanel', 'birth_date': '1855-02-13', 'death_date': '1922-04-28', 'place_of_birth': 'Schaerbeek - Schaarbeek', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Paul_Deschanel', 'start_mandate': '1920-02-18', 'end_mandate': '1920-09-21'}</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q312026', 'first_name': 'Georges', 'last_name': 'Bidault', 'birth_date': '1899-10-05', 'death_date': '1983-01-27', 'place_of_birth': 'Moulins', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Georges_Bidault', 'start_mandate': '1946-06-24', 'end_mandate': '1946-10-14'}</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q315656', 'first_name': 'Jean', 'last_name': 'Casimir-Perier', 'birth_date': '1847-11-08', 'death_date': '1907-03-11', 'place_of_birth': 'Paris', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Jean_Casimir-Perier', 'start_mandate': '1894-06-27', 'end_mandate': '1895-01-16'}</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q356032', 'first_name': 'Charles', 'last_name': 'Dupuy', 'birth_date': '1851-11-05', 'death_date': '1923-07-23', 'place_of_birth': 'Le Puy-en-Velay', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Charles_Dupuy', 'start_mandate': '1894-06-25', 'end_mandate': '1894-06-27'}</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q379702', 'first_name': 'Louis', 'last_name': 'Cavaignac', 'birth_date': '1802-10-15', 'death_date': '1857-10-28', 'place_of_birth': 'Paris', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Eug%C3%A8ne_Cavaignac', 'start_mandate': '1848-06-28', 'end_mandate': '1848-12-20'}</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q441235', 'first_name': 'Louis', 'last_name': 'None', 'birth_date': '1815-03-12', 'death_date': '1896-10-07', 'place_of_birth': 'Le Palais', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Louis_Jules_Trochu', 'start_mandate': '1870-09-04', 'end_mandate': '1871-01-22'}</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q459212', 'first_name': 'Frédéric', 'last_name': 'None', 'birth_date': '1874-03-16', 'death_date': '1958-05-20', 'place_of_birth': 'Paris', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Fr%C3%A9d%C3%A9ric_Fran%C3%A7ois-Marsal', 'start_mandate': '1924-06-11', 'end_mandate': '1924-06-13'}</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>{'id': 'Q3052772', 'first_name': 'Emmanuel', 'last_name': 'Macron', 'birth_date': '1977-12-21', 'death_date': None, 'place_of_birth': 'Amiens', 'wikipedia_url': 'https://fr.wikipedia.org/wiki/Emmanuel_Macron', 'start_mandate': '2017-05-14', 'end_mandate': None}</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="inlineStr"/>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="inlineStr"/>
+      <c r="BA3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -595,55 +1052,73 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Q193874</t>
+          <t>{'id': 'Q57553', 'first_name': 'Mohammed', 'last_name': 'None', 'birth_date': '1963-08-21', 'death_date': None, 'place_of_birth': 'Rabat', 'wikipedia_url': 'https://ar.wikipedia.org/wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%B3%D8%A7%D8%AF%D8%B3_%D8%A8%D9%86_%D8%A7%D9%84%D8%AD%D8%B3%D9%86', 'start_mandate': '1999-07-23', 'end_mandate': None}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mohammed</t>
+          <t>{'id': 'Q69103', 'first_name': 'Hassan', 'last_name': 'None', 'birth_date': '1929-07-09', 'death_date': '1999-07-20', 'place_of_birth': 'Rabat', 'wikipedia_url': 'https://ar.wikipedia.org/wiki/%D8%A7%D9%84%D8%AD%D8%B3%D9%86_%D8%A7%D9%84%D8%AB%D8%A7%D9%86%D9%8A_%D8%A8%D9%86_%D9%85%D8%AD%D9%85%D8%AF', 'start_mandate': '1961-02-26', 'end_mandate': '1999-07-23'}</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>{'id': 'Q193874', 'first_name': 'Mohammed', 'last_name': 'None', 'birth_date': '1909-08-10', 'death_date': '1961-02-26', 'place_of_birth': 'Fez', 'wikipedia_url': 'https://ar.wikipedia.org/wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%AE%D8%A7%D9%85%D8%B3_%D8%A8%D9%86_%D9%8A%D9%88%D8%B3%D9%81', 'start_mandate': '1957-08-14', 'end_mandate': '1961-02-26'}</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1909-08-10</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1961-02-26</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Fez</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>https://ar.wikipedia.org/wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%AE%D8%A7%D9%85%D8%B3_%D8%A8%D9%86_%D9%8A%D9%88%D8%B3%D9%81</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1957-08-14</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>1961-02-26</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">محمد الخامس بن يوسف بن الحسن بن محمد بن عبد الرحمن بن هشام بن محمد بن عبد الله بن إسماعيل بن إسماعيل بن الشريف بن علي العلوي ولد وتوفي خلف والده السلطان مولاي يوسف الذي توفي بكرة يوم الخميس 22 جمادى الأولى سنة 1346 هـ موافق 17 نوفمبر سنة 1927م فبويع ابنه سيدي محمد سلطانا للمغرب في اليوم الموالي بعد صلاة الجمعة 23 جمادى الأولى سنة 1346 هـ موافق 18 نوفمبر سنة 1927م في القصر السلطاني بفاس ولم يزل سلطان المغرب إلى سنة 1957م قضى منها المنفى بين ثم اتخذ لقب الملك سنة 1957م ولم يزل ملكا إلى وفاته سنة 1961م ساند السلطان محمد الخامس نضالات الحركة الوطنية المغربية المطالبة بتحقيق الاستقلال الشيء الذي دفعه إلى الاصطدام بسلطات الحماية. وكانت النتيجة قيام سلطات الحماية بنفيه إلى مدغشقر. وعلى إثر ذلك اندلعت مظاهرات مطالبة بعودته إلى وطنه. وأمام اشتداد حدة المظاهرات قبلت السلطات الفرنسية بإرجاع السلطان إلى عرشه يوم 16 نوفمبر 1955. وبعد بضعة شهور تم إعلان استقلال المغرب. كان الملك محمد الخامس يكنى أبا عبد الله.
-</t>
-        </is>
-      </c>
+          <t>{'id': 'Q334782', 'first_name': 'Mohammed', 'last_name': 'None', 'birth_date': None, 'death_date': None, 'place_of_birth': 'None', 'wikipedia_url': 'https://ar.wikipedia.org/wiki/%D8%A7%D9%84%D9%82%D8%A7%D8%A6%D9%85_%D8%A8%D8%A3%D9%85%D8%B1_%D8%A7%D9%84%D9%84%D9%87_%D8%A7%D9%84%D8%B3%D8%B9%D8%AF%D9%8A', 'start_mandate': None, 'end_mandate': '1517-01-01'}</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -651,43 +1126,307 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Q334782</t>
+          <t>{'id': 'Q7747', 'first_name': 'Vladimir', 'last_name': 'Putin', 'birth_date': '1952-10-07', 'death_date': None, 'place_of_birth': 'Saint Petersburg', 'wikipedia_url': 'https://ru.wikipedia.org/wiki/%D0%9F%D1%83%D1%82%D0%B8%D0%BD,_%D0%92%D0%BB%D0%B0%D0%B4%D0%B8%D0%BC%D0%B8%D1%80_%D0%92%D0%BB%D0%B0%D0%B4%D0%B8%D0%BC%D0%B8%D1%80%D0%BE%D0%B2%D0%B8%D1%87', 'start_mandate': '2000-05-07', 'end_mandate': '2008-05-07'}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mohammed</t>
+          <t>{'id': 'Q23530', 'first_name': 'Dmitry', 'last_name': 'Medvedev', 'birth_date': '1965-09-14', 'death_date': None, 'place_of_birth': 'Saint Petersburg', 'wikipedia_url': 'https://ru.wikipedia.org/wiki/%D0%9C%D0%B5%D0%B4%D0%B2%D0%B5%D0%B4%D0%B5%D0%B2,_%D0%94%D0%BC%D0%B8%D1%82%D1%80%D0%B8%D0%B9_%D0%90%D0%BD%D0%B0%D1%82%D0%BE%D0%BB%D1%8C%D0%B5%D0%B2%D0%B8%D1%87', 'start_mandate': '2008-05-07', 'end_mandate': '2012-05-07'}</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>{'id': 'Q34453', 'first_name': 'Boris', 'last_name': 'Yeltsin', 'birth_date': '1931-02-01', 'death_date': '2007-04-23', 'place_of_birth': 'Butka', 'wikipedia_url': 'https://ru.wikipedia.org/wiki/%D0%95%D0%BB%D1%8C%D1%86%D0%B8%D0%BD,_%D0%91%D0%BE%D1%80%D0%B8%D1%81_%D0%9D%D0%B8%D0%BA%D0%BE%D0%BB%D0%B0%D0%B5%D0%B2%D0%B8%D1%87', 'start_mandate': '1991-07-10', 'end_mandate': '1999-12-31'}</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>https://ar.wikipedia.org/wiki/%D8%A7%D9%84%D9%82%D8%A7%D8%A6%D9%85_%D8%A8%D8%A3%D9%85%D8%B1_%D8%A7%D9%84%D9%84%D9%87_%D8%A7%D9%84%D8%B3%D8%B9%D8%AF%D9%8A</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>1517-01-01</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">أبو عبد الله محمد بن محمد ابن علي بن مخلوف بن زيدان الملقب بالقائم بأمر الله عميد الأسرة السعدية وأول سلطان للمغرب من الأسرة السعدية حكم بين 1509 - 1517.
-</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="inlineStr"/>
+      <c r="AW5" t="inlineStr"/>
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="inlineStr"/>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q23', 'first_name': 'George', 'last_name': 'Washington', 'birth_date': '1732-02-22', 'death_date': '1799-12-14', 'place_of_birth': 'Westmoreland County', 'wikipedia_url': 'https://en.wikipedia.org/wiki/George_Washington', 'start_mandate': '1789-04-30', 'end_mandate': '1797-03-04'}</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q76', 'first_name': 'Barack', 'last_name': 'Obama', 'birth_date': '1961-08-04', 'death_date': None, 'place_of_birth': 'Kapiolani Medical Center for Women and Children', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Barack_Obama', 'start_mandate': '2009-01-20', 'end_mandate': '2017-01-20'}</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q91', 'first_name': 'Abraham', 'last_name': 'Lincoln', 'birth_date': '1809-02-12', 'death_date': '1865-04-15', 'place_of_birth': 'Sinking Spring Farm', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Abraham_Lincoln', 'start_mandate': '1861-03-04', 'end_mandate': '1865-04-15'}</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q207', 'first_name': 'George', 'last_name': 'Bush', 'birth_date': '1946-07-06', 'death_date': None, 'place_of_birth': 'New Haven', 'wikipedia_url': 'https://en.wikipedia.org/wiki/George_W._Bush', 'start_mandate': '2001-01-20', 'end_mandate': '2009-01-20'}</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q1124', 'first_name': 'Bill', 'last_name': 'Clinton', 'birth_date': '1946-08-19', 'death_date': None, 'place_of_birth': 'Hope', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Bill_Clinton', 'start_mandate': '1993-01-20', 'end_mandate': '2001-01-20'}</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q6279', 'first_name': 'Joe', 'last_name': 'Biden', 'birth_date': '1942-11-20', 'death_date': None, 'place_of_birth': "St. Mary's Hospital", 'wikipedia_url': 'https://en.wikipedia.org/wiki/Joe_Biden', 'start_mandate': '2021-01-20', 'end_mandate': None}</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q8007', 'first_name': 'Franklin', 'last_name': 'Roosevelt', 'birth_date': '1882-01-30', 'death_date': '1945-04-12', 'place_of_birth': 'Hyde Park', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Franklin_D._Roosevelt', 'start_mandate': '1933-03-04', 'end_mandate': '1945-04-12'}</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q8612', 'first_name': 'Andrew', 'last_name': 'Johnson', 'birth_date': '1808-12-29', 'death_date': '1875-07-31', 'place_of_birth': 'Raleigh', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Andrew_Johnson', 'start_mandate': '1865-04-15', 'end_mandate': '1869-03-04'}</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q9582', 'first_name': 'Gerald', 'last_name': 'Ford', 'birth_date': '1913-07-14', 'death_date': '2006-12-26', 'place_of_birth': 'Omaha', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Gerald_Ford', 'start_mandate': '1974-08-09', 'end_mandate': '1977-01-20'}</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q9588', 'first_name': 'Richard', 'last_name': 'Nixon', 'birth_date': '1913-01-09', 'death_date': '1994-04-22', 'place_of_birth': 'Yorba Linda', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Richard_Nixon', 'start_mandate': '1969-01-20', 'end_mandate': '1974-08-09'}</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q9640', 'first_name': 'Lyndon', 'last_name': 'Johnson', 'birth_date': '1908-08-27', 'death_date': '1973-01-22', 'place_of_birth': 'Stonewall', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Lyndon_B._Johnson', 'start_mandate': '1963-11-22', 'end_mandate': '1969-01-20'}</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q9696', 'first_name': 'John', 'last_name': 'Kennedy', 'birth_date': '1917-05-29', 'death_date': '1963-11-22', 'place_of_birth': 'Brookline', 'wikipedia_url': 'https://en.wikipedia.org/wiki/John_F._Kennedy', 'start_mandate': '1961-01-20', 'end_mandate': '1963-11-22'}</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q9916', 'first_name': 'Dwight', 'last_name': 'Eisenhower', 'birth_date': '1890-10-14', 'death_date': '1969-03-28', 'place_of_birth': 'Denison', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Dwight_D._Eisenhower', 'start_mandate': '1953-01-20', 'end_mandate': '1961-01-20'}</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q9960', 'first_name': 'Ronald', 'last_name': 'Reagan', 'birth_date': '1911-02-06', 'death_date': '2004-06-05', 'place_of_birth': 'Tampico', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Ronald_Reagan', 'start_mandate': '1981-01-20', 'end_mandate': '1989-01-20'}</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11613', 'first_name': 'Harry', 'last_name': 'Truman', 'birth_date': '1884-05-08', 'death_date': '1972-12-26', 'place_of_birth': 'Lamar', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Harry_S._Truman', 'start_mandate': '1945-04-12', 'end_mandate': '1953-01-20'}</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11806', 'first_name': 'John', 'last_name': 'Adams', 'birth_date': None, 'death_date': '1826-07-04', 'place_of_birth': 'Braintree', 'wikipedia_url': 'https://en.wikipedia.org/wiki/John_Adams', 'start_mandate': '1797-03-04', 'end_mandate': '1801-03-04'}</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11812', 'first_name': 'Thomas', 'last_name': 'Jefferson', 'birth_date': None, 'death_date': '1826-07-04', 'place_of_birth': 'Shadwell', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Thomas_Jefferson', 'start_mandate': '1801-03-04', 'end_mandate': '1809-03-04'}</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11813', 'first_name': 'James', 'last_name': 'Madison', 'birth_date': '1751-03-16', 'death_date': '1836-06-28', 'place_of_birth': 'Port Conway', 'wikipedia_url': 'https://en.wikipedia.org/wiki/James_Madison', 'start_mandate': '1809-03-04', 'end_mandate': '1817-03-04'}</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11815', 'first_name': 'James', 'last_name': 'Monroe', 'birth_date': '1758-04-28', 'death_date': '1831-07-04', 'place_of_birth': 'Monroe Hall', 'wikipedia_url': 'https://en.wikipedia.org/wiki/James_Monroe', 'start_mandate': '1817-03-04', 'end_mandate': '1825-03-04'}</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11816', 'first_name': 'John', 'last_name': 'Adams', 'birth_date': '1767-07-11', 'death_date': '1848-02-23', 'place_of_birth': 'Braintree', 'wikipedia_url': 'https://en.wikipedia.org/wiki/John_Quincy_Adams', 'start_mandate': '1825-03-04', 'end_mandate': '1829-03-04'}</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11817', 'first_name': 'Andrew', 'last_name': 'Jackson', 'birth_date': '1767-03-15', 'death_date': '1845-06-08', 'place_of_birth': 'Waxhaws', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Andrew_Jackson', 'start_mandate': '1829-03-04', 'end_mandate': '1837-03-04'}</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11820', 'first_name': 'Martin', 'last_name': 'Van Buren', 'birth_date': '1782-12-05', 'death_date': '1862-07-24', 'place_of_birth': 'Kinderhook', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Martin_Van_Buren', 'start_mandate': '1837-03-04', 'end_mandate': '1841-03-04'}</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11869', 'first_name': 'William', 'last_name': 'Harrison', 'birth_date': '1773-02-09', 'death_date': '1841-04-04', 'place_of_birth': 'Charles City County', 'wikipedia_url': 'https://en.wikipedia.org/wiki/William_Henry_Harrison', 'start_mandate': '1841-03-04', 'end_mandate': '1841-04-04'}</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11881', 'first_name': 'John', 'last_name': 'Tyler', 'birth_date': '1790-03-29', 'death_date': '1862-01-18', 'place_of_birth': 'Charles City County', 'wikipedia_url': 'https://en.wikipedia.org/wiki/John_Tyler', 'start_mandate': '1841-04-04', 'end_mandate': '1845-03-04'}</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11891', 'first_name': 'James', 'last_name': 'Polk', 'birth_date': '1795-11-02', 'death_date': '1849-06-15', 'place_of_birth': 'Pineville', 'wikipedia_url': 'https://en.wikipedia.org/wiki/James_K._Polk', 'start_mandate': '1845-03-04', 'end_mandate': '1849-03-04'}</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q11896', 'first_name': 'Zachary', 'last_name': 'Taylor', 'birth_date': '1784-11-24', 'death_date': '1850-07-09', 'place_of_birth': 'Barboursville', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Zachary_Taylor', 'start_mandate': '1849-03-04', 'end_mandate': '1850-07-09'}</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q12306', 'first_name': 'Millard', 'last_name': 'Fillmore', 'birth_date': '1800-01-07', 'death_date': '1874-03-08', 'place_of_birth': 'Summerhill', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Millard_Fillmore', 'start_mandate': '1850-07-09', 'end_mandate': '1853-03-04'}</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q12312', 'first_name': 'Franklin', 'last_name': 'Pierce', 'birth_date': '1804-11-23', 'death_date': '1869-10-08', 'place_of_birth': 'Hillsborough', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Franklin_Pierce', 'start_mandate': '1853-03-04', 'end_mandate': '1857-03-04'}</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q12325', 'first_name': 'James', 'last_name': 'Buchanan', 'birth_date': '1791-04-23', 'death_date': '1868-06-01', 'place_of_birth': 'Stony Batter', 'wikipedia_url': 'https://en.wikipedia.org/wiki/James_Buchanan', 'start_mandate': '1857-03-04', 'end_mandate': '1861-03-04'}</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q22686', 'first_name': 'Donald', 'last_name': 'Trump', 'birth_date': '1946-06-14', 'death_date': None, 'place_of_birth': 'Jamaica Hospital Medical Center', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Donald_Trump', 'start_mandate': '2017-01-20', 'end_mandate': '2021-01-20'}</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q23505', 'first_name': 'George', 'last_name': 'Bush', 'birth_date': '1924-06-12', 'death_date': '2018-11-30', 'place_of_birth': 'Milton', 'wikipedia_url': 'https://en.wikipedia.org/wiki/George_H._W._Bush', 'start_mandate': '1989-01-20', 'end_mandate': '1993-01-20'}</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q23685', 'first_name': 'Jimmy', 'last_name': 'Carter', 'birth_date': '1924-10-01', 'death_date': None, 'place_of_birth': 'Lillian G. Carter Nursing Center', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Jimmy_Carter', 'start_mandate': '1977-01-20', 'end_mandate': '1981-01-20'}</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q33866', 'first_name': 'Theodore', 'last_name': 'Roosevelt', 'birth_date': '1858-10-27', 'death_date': '1919-01-06', 'place_of_birth': 'Manhattan', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Theodore_Roosevelt', 'start_mandate': '1901-09-14', 'end_mandate': '1909-03-04'}</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q34296', 'first_name': 'Woodrow', 'last_name': 'Wilson', 'birth_date': '1856-12-28', 'death_date': '1924-02-03', 'place_of_birth': 'Staunton', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Woodrow_Wilson', 'start_mandate': '1913-03-04', 'end_mandate': '1921-03-04'}</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q34597', 'first_name': 'James', 'last_name': 'Garfield', 'birth_date': '1831-11-19', 'death_date': '1881-09-19', 'place_of_birth': 'Moreland Hills', 'wikipedia_url': 'https://en.wikipedia.org/wiki/James_A._Garfield', 'start_mandate': '1881-03-04', 'end_mandate': '1881-09-19'}</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q34836', 'first_name': 'Ulysses', 'last_name': 'Grant', 'birth_date': '1822-04-27', 'death_date': '1885-07-23', 'place_of_birth': 'Point Pleasant', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Ulysses_S._Grant', 'start_mandate': '1869-03-04', 'end_mandate': '1877-03-04'}</t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q35041', 'first_name': 'William', 'last_name': 'McKinley', 'birth_date': '1843-01-29', 'death_date': '1901-09-14', 'place_of_birth': 'Niles', 'wikipedia_url': 'https://en.wikipedia.org/wiki/William_McKinley', 'start_mandate': '1897-03-04', 'end_mandate': '1901-09-14'}</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q35171', 'first_name': 'Stephen', 'last_name': 'Cleveland', 'birth_date': '1837-03-18', 'death_date': '1908-06-24', 'place_of_birth': 'Caldwell', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Grover_Cleveland', 'start_mandate': '1893-03-04', 'end_mandate': '1897-03-04'}</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q35236', 'first_name': 'Herbert', 'last_name': 'Hoover', 'birth_date': '1874-08-10', 'death_date': '1964-10-20', 'place_of_birth': 'West Branch', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Herbert_Hoover', 'start_mandate': '1929-03-04', 'end_mandate': '1933-03-04'}</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q35286', 'first_name': 'Warren', 'last_name': 'Harding', 'birth_date': '1865-11-02', 'death_date': '1923-08-02', 'place_of_birth': 'Blooming Grove', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Warren_G._Harding', 'start_mandate': '1921-03-04', 'end_mandate': '1923-08-02'}</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q35498', 'first_name': 'Chester', 'last_name': 'Arthur', 'birth_date': '1829-10-05', 'death_date': '1886-11-18', 'place_of_birth': 'Fairfield', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Chester_A._Arthur', 'start_mandate': '1881-09-19', 'end_mandate': '1885-03-04'}</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q35648', 'first_name': 'William', 'last_name': 'Taft', 'birth_date': '1857-09-15', 'death_date': '1930-03-08', 'place_of_birth': 'Cincinnati', 'wikipedia_url': 'https://en.wikipedia.org/wiki/William_Howard_Taft', 'start_mandate': '1909-03-04', 'end_mandate': '1913-03-04'}</t>
+        </is>
+      </c>
+      <c r="AR6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q35678', 'first_name': 'Benjamin', 'last_name': 'Harrison', 'birth_date': '1833-08-20', 'death_date': '1901-03-13', 'place_of_birth': 'North Bend', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Benjamin_Harrison', 'start_mandate': '1889-03-04', 'end_mandate': '1893-03-04'}</t>
+        </is>
+      </c>
+      <c r="AS6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q35686', 'first_name': 'Rutherford', 'last_name': 'Hayes', 'birth_date': '1822-10-04', 'death_date': '1893-01-17', 'place_of_birth': 'Delaware', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Rutherford_B._Hayes', 'start_mandate': '1877-03-04', 'end_mandate': '1881-03-04'}</t>
+        </is>
+      </c>
+      <c r="AT6" t="inlineStr">
+        <is>
+          <t>{'id': 'Q36023', 'first_name': 'John', 'last_name': 'Coolidge', 'birth_date': '1872-07-04', 'death_date': '1933-01-05', 'place_of_birth': 'Plymouth Notch', 'wikipedia_url': 'https://en.wikipedia.org/wiki/Calvin_Coolidge', 'start_mandate': '1923-08-02', 'end_mandate': '1929-03-04'}</t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="inlineStr"/>
+      <c r="AW6" t="inlineStr"/>
+      <c r="AX6" t="inlineStr"/>
+      <c r="AY6" t="inlineStr"/>
+      <c r="AZ6" t="inlineStr"/>
+      <c r="BA6" t="inlineStr"/>
+      <c r="BB6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated main, json parsing
</commit_message>
<xml_diff>
--- a/leaders.xlsx
+++ b/leaders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,6 +689,166 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Q7747</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Vladimir</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Putin</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1952-10-07</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Saint Petersburg</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://ru.wikipedia.org/wiki/%D0%9F%D1%83%D1%82%D0%B8%D0%BD,_%D0%92%D0%BB%D0%B0%D0%B4%D0%B8%D0%BC%D0%B8%D1%80_%D0%92%D0%BB%D0%B0%D0%B4%D0%B8%D0%BC%D0%B8%D1%80%D0%BE%D0%B2%D0%B8%D1%87</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2000-05-07</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2008-05-07</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Владимир Владимирович Путин российский государственный и политический деятель. Действующий президент Российской Федерации, председатель Государственного Совета Российской Федерации и Совета Безопасности Российской Федерации Верховный главнокомандующий Вооружёнными силами Российской Федерации с 7 мая 2012 года. Ранее занимал должность президента с 7 мая 2000 по 7 мая 2008 года, также в 19992000 и 20082012 годах занимал должность председателя правительства Российской Федерации. Фактически руководит Россией, согласно разным оценкам, с 1999 или с 2000 года. В сентябре 2017 года Путин стал самым долго правящим российским лидером со времён Иосифа Сталина.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Q23530</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Dmitry</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Medvedev</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1965-09-14</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Saint Petersburg</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://ru.wikipedia.org/wiki/%D0%9C%D0%B5%D0%B4%D0%B2%D0%B5%D0%B4%D0%B5%D0%B2,_%D0%94%D0%BC%D0%B8%D1%82%D1%80%D0%B8%D0%B9_%D0%90%D0%BD%D0%B0%D1%82%D0%BE%D0%BB%D1%8C%D0%B5%D0%B2%D0%B8%D1%87</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2008-05-07</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2012-05-07</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">иностранные
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Q34453</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Boris</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Yeltsin</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1931-02-01</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2007-04-23</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Butka</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://ru.wikipedia.org/wiki/%D0%95%D0%BB%D1%8C%D1%86%D0%B8%D0%BD,_%D0%91%D0%BE%D1%80%D0%B8%D1%81_%D0%9D%D0%B8%D0%BA%D0%BE%D0%BB%D0%B0%D0%B5%D0%B2%D0%B8%D1%87</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1991-07-10</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>1999-12-31</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Борис Николаевич Ельцин, Бутка, Буткинский район, Уральская область, СССР 23 апреля 2007, Москва, Россия советский и российский партийный, государственный и политический деятель, первый всенародно избранный Президент Российской Федерации в ноябре 1991 июне 1992 года одновременно возглавлял правительство. С марта по май 1992 года исполнял обязанности министра обороны Российской Федерации.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>